<commit_message>
Update data flows and reports
</commit_message>
<xml_diff>
--- a/tags.xlsx
+++ b/tags.xlsx
@@ -14,9 +14,249 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Element</t>
+  </si>
+  <si>
+    <t>argocd</t>
+  </si>
+  <si>
+    <t>kubernetes</t>
+  </si>
+  <si>
+    <t>redis</t>
+  </si>
+  <si>
+    <t>API Server</t>
+  </si>
+  <si>
+    <t>Validate External OIDC Token</t>
+  </si>
+  <si>
+    <t>Validate Dex OIDC Token</t>
+  </si>
+  <si>
+    <t>Update Repo Access Credentials</t>
+  </si>
+  <si>
+    <t>Update RBAC Config</t>
+  </si>
+  <si>
+    <t>Update Cluster Access Config</t>
+  </si>
+  <si>
+    <t>Pull Argo CD Image</t>
+  </si>
+  <si>
+    <t>Get/Update/Delete Live Resource State from Kubernetes (Host)</t>
+  </si>
+  <si>
+    <t>Get/Update/Delete Live Resource State from Kubernetes (External)</t>
+  </si>
+  <si>
+    <t>Fetching Rendered Manifests from Cache</t>
+  </si>
+  <si>
+    <t>Application Controller</t>
+  </si>
+  <si>
+    <t>Rendered Manifest Requests</t>
+  </si>
+  <si>
+    <t>Reconcile Resource State (Host Cluster)</t>
+  </si>
+  <si>
+    <t>Reconcile Resource State (External Cluster)</t>
+  </si>
+  <si>
+    <t>ApplicationSet Controller</t>
+  </si>
+  <si>
+    <t>Git Generator Pull</t>
+  </si>
+  <si>
+    <t>Argo CD Build Pipeline (GitHub Actions)</t>
+  </si>
+  <si>
+    <t>Push Image to Quay</t>
+  </si>
+  <si>
+    <t>Pull Source</t>
+  </si>
+  <si>
+    <t>Pull Base Image from Docker Hub</t>
+  </si>
+  <si>
+    <t>Argo CD Maintainer Git Client</t>
+  </si>
+  <si>
+    <t>Push Code/Tags to GitHub</t>
+  </si>
+  <si>
+    <t>Argo CD Source Repo (GitHub)</t>
+  </si>
+  <si>
+    <t>Docker Hub</t>
+  </si>
+  <si>
+    <t>External Cluster Kubernetes API</t>
+  </si>
+  <si>
+    <t>Host Cluster Kubernetes API</t>
+  </si>
+  <si>
+    <t>Internal Source Control Management API</t>
+  </si>
+  <si>
+    <t>Internal Source Control Management UI</t>
+  </si>
+  <si>
+    <t>Push Manifest Sources</t>
+  </si>
+  <si>
+    <t>OIDC Provider (External)</t>
+  </si>
+  <si>
+    <t>OIDC Proxy (Dex)</t>
+  </si>
+  <si>
+    <t>Proxying to an External OIDC Provider</t>
+  </si>
+  <si>
+    <t>Quay</t>
+  </si>
+  <si>
+    <t>Rendered Manifests Cache (Redis)</t>
+  </si>
+  <si>
+    <t>Repo Server</t>
+  </si>
+  <si>
+    <t>Store Cached Manifest Sources</t>
+  </si>
+  <si>
+    <t>Send/Receive Cached Rendered Manifests</t>
+  </si>
+  <si>
+    <t>Get Repo Access Credentials</t>
+  </si>
+  <si>
+    <t>Fetch Manifest Sources</t>
+  </si>
+  <si>
+    <t>Repo Server Storage</t>
+  </si>
+  <si>
+    <t>User CLI</t>
+  </si>
+  <si>
+    <t>Make Requests to API Server</t>
+  </si>
+  <si>
+    <t>API Server Secret</t>
+  </si>
+  <si>
+    <t>AppProject Manifest</t>
+  </si>
+  <si>
+    <t>Application Manifest</t>
+  </si>
+  <si>
+    <t>Application Name</t>
+  </si>
+  <si>
+    <t>ApplicationSet Manifest</t>
+  </si>
+  <si>
+    <t>ApplicationSet Name</t>
+  </si>
+  <si>
+    <t>Argo CD Base Image</t>
+  </si>
+  <si>
+    <t>Argo CD Container Image</t>
+  </si>
+  <si>
+    <t>Argo CD Container Image Tag</t>
+  </si>
+  <si>
+    <t>Argo CD Database Export</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Argo CD GitHub Push Token</t>
+  </si>
+  <si>
+    <t>Argo CD RBAC Config</t>
+  </si>
+  <si>
+    <t>Argo CD Source</t>
+  </si>
+  <si>
+    <t>Argo CD User Provided Secret</t>
+  </si>
+  <si>
+    <t>Argo Tokens</t>
+  </si>
+  <si>
+    <t>Cluster Access Configuration</t>
+  </si>
+  <si>
+    <t>Cluster Access Credentials</t>
+  </si>
+  <si>
+    <t>Git Branch Name</t>
+  </si>
+  <si>
+    <t>Git Organization Name</t>
+  </si>
+  <si>
+    <t>Git Repo Name</t>
+  </si>
+  <si>
+    <t>Git Repo URL</t>
+  </si>
+  <si>
+    <t>Live Manifests</t>
+  </si>
+  <si>
+    <t>Manifest Sources</t>
+  </si>
+  <si>
+    <t>OIDC Public Keys</t>
+  </si>
+  <si>
+    <t>OIDC Tokens</t>
+  </si>
+  <si>
+    <t>Quay Push Token</t>
+  </si>
+  <si>
+    <t>Rendered Manifests</t>
+  </si>
+  <si>
+    <t>Repo Access Credentials</t>
+  </si>
+  <si>
+    <t>Build Time Boundary</t>
+  </si>
+  <si>
+    <t>External Services</t>
+  </si>
+  <si>
+    <t>Kubernetes Argo CD Namespace</t>
+  </si>
+  <si>
+    <t>Kubernetes Network</t>
+  </si>
+  <si>
+    <t>Organization Network</t>
+  </si>
+  <si>
+    <t>Kubernetes Node</t>
   </si>
 </sst>
 </file>
@@ -379,6 +619,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
+    <col customWidth="true" max="2" min="2" width="35"/>
+    <col customWidth="true" max="3" min="3" width="35"/>
+    <col customWidth="true" max="4" min="4" width="35"/>
     <col customWidth="true" max="1" min="1" width="60"/>
   </cols>
   <sheetData>
@@ -386,6 +629,663 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="1"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
     </row>
   </sheetData>
   <pageSetup orientation="landscape" paperSize="9"/>

</xml_diff>

<commit_message>
add web UI, tweak some details
format
</commit_message>
<xml_diff>
--- a/tags.xlsx
+++ b/tags.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Element</t>
   </si>
@@ -157,6 +157,12 @@
     <t>Make Requests to API Server</t>
   </si>
   <si>
+    <t>Web UI</t>
+  </si>
+  <si>
+    <t>Get App Code</t>
+  </si>
+  <si>
     <t>API Server Secret</t>
   </si>
   <si>
@@ -205,6 +211,9 @@
     <t>Argo Tokens</t>
   </si>
   <si>
+    <t>Bundled UI Code</t>
+  </si>
+  <si>
     <t>Cluster Access Configuration</t>
   </si>
   <si>
@@ -227,6 +236,12 @@
   </si>
   <si>
     <t>Manifest Sources</t>
+  </si>
+  <si>
+    <t>OIDC Client Secret</t>
+  </si>
+  <si>
+    <t>OIDC Configuration</t>
   </si>
   <si>
     <t>OIDC Public Keys</t>
@@ -1028,7 +1043,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1036,7 +1051,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1044,7 +1059,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1052,7 +1067,7 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1060,7 +1075,7 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1068,7 +1083,7 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1076,7 +1091,7 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1084,7 +1099,7 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1092,21 +1107,15 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1114,7 +1123,7 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1122,25 +1131,29 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1"/>
-      <c r="C62" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1148,7 +1161,7 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1156,15 +1169,17 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="C65" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D65" s="1"/>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1172,7 +1187,7 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1180,7 +1195,7 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1188,7 +1203,7 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1196,7 +1211,7 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1204,7 +1219,7 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1212,7 +1227,7 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1220,7 +1235,7 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1228,7 +1243,7 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1236,7 +1251,7 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1244,7 +1259,7 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1252,7 +1267,7 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1260,7 +1275,7 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1268,7 +1283,7 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1276,7 +1291,7 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1284,7 +1299,7 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1292,11 +1307,59 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
     </row>
   </sheetData>
   <pageSetup orientation="landscape" paperSize="9"/>

</xml_diff>

<commit_message>
address risks, sort keys
</commit_message>
<xml_diff>
--- a/tags.xlsx
+++ b/tags.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Element</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Application Controller</t>
-  </si>
-  <si>
-    <t>Rendered Manifest Requests</t>
   </si>
   <si>
     <t>Reconcile Resource State (Host Cluster)</t>
@@ -805,7 +802,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -813,7 +810,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -821,7 +818,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -829,7 +826,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -837,7 +834,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -845,7 +842,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -853,7 +850,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -861,7 +858,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -869,7 +866,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -877,7 +874,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -885,7 +882,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -893,7 +890,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -901,7 +898,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -909,7 +906,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -917,7 +914,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -925,7 +922,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -933,7 +930,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -941,7 +938,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -949,7 +946,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -957,7 +954,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -965,7 +962,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -973,7 +970,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -981,7 +978,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -989,7 +986,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -997,7 +994,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1005,7 +1002,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1013,7 +1010,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1021,7 +1018,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1029,7 +1026,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1037,7 +1034,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1045,7 +1042,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1053,7 +1050,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1061,7 +1058,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1069,7 +1066,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1077,7 +1074,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1085,7 +1082,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1093,7 +1090,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1101,7 +1098,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1109,7 +1106,7 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1117,7 +1114,7 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1125,7 +1122,7 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1133,7 +1130,7 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1141,7 +1138,7 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1149,7 +1146,7 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1157,7 +1154,7 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1165,7 +1162,7 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1173,7 +1170,7 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1181,7 +1178,7 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1189,7 +1186,7 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1197,7 +1194,7 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1205,7 +1202,7 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1213,7 +1210,7 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1221,7 +1218,7 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1229,21 +1226,21 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1251,7 +1248,7 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1259,7 +1256,7 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1267,17 +1264,17 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D72" s="1"/>
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1285,7 +1282,7 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1293,7 +1290,7 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1301,7 +1298,7 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1309,7 +1306,7 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1317,7 +1314,7 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1325,7 +1322,7 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1333,7 +1330,7 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1341,7 +1338,7 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1349,7 +1346,7 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1357,7 +1354,7 @@
     </row>
     <row r="83">
       <c r="A83" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1365,7 +1362,7 @@
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1373,7 +1370,7 @@
     </row>
     <row r="85">
       <c r="A85" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1381,7 +1378,7 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1389,7 +1386,7 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1397,7 +1394,7 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1405,7 +1402,7 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1413,7 +1410,7 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1421,7 +1418,7 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1429,7 +1426,7 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1437,7 +1434,7 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1445,7 +1442,7 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1453,7 +1450,7 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1461,7 +1458,7 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1469,7 +1466,7 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1477,7 +1474,7 @@
     </row>
     <row r="98">
       <c r="A98" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1485,7 +1482,7 @@
     </row>
     <row r="99">
       <c r="A99" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1493,7 +1490,7 @@
     </row>
     <row r="100">
       <c r="A100" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>

</xml_diff>